<commit_message>
finished second model eval
</commit_message>
<xml_diff>
--- a/Export/FeatureImportance_Summary.xlsx
+++ b/Export/FeatureImportance_Summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>feature</t>
   </si>
@@ -25,142 +25,115 @@
     <t>Model</t>
   </si>
   <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>pi_std</t>
+  </si>
+  <si>
+    <t>sstk_std</t>
+  </si>
+  <si>
+    <t>ivncf</t>
+  </si>
+  <si>
+    <t>sec_trt1m_std</t>
+  </si>
+  <si>
+    <t>seq</t>
+  </si>
+  <si>
+    <t>teq</t>
+  </si>
+  <si>
+    <t>sstk</t>
+  </si>
+  <si>
+    <t>rest_sum_diff</t>
+  </si>
+  <si>
+    <t>ppegt</t>
+  </si>
+  <si>
+    <t>caps</t>
+  </si>
+  <si>
+    <t>xopr</t>
+  </si>
+  <si>
+    <t>fopo_std</t>
+  </si>
+  <si>
+    <t>spce_std</t>
+  </si>
+  <si>
+    <t>ceq</t>
+  </si>
+  <si>
+    <t>ceqt</t>
+  </si>
+  <si>
+    <t>spce</t>
+  </si>
+  <si>
+    <t>cshpri</t>
+  </si>
+  <si>
+    <t>ceq_std</t>
+  </si>
+  <si>
+    <t>tstk</t>
+  </si>
+  <si>
+    <t>cogs</t>
+  </si>
+  <si>
+    <t>revt</t>
+  </si>
+  <si>
+    <t>icapt</t>
+  </si>
+  <si>
+    <t>rest_count</t>
+  </si>
+  <si>
+    <t>cogs_std</t>
+  </si>
+  <si>
+    <t>rest_a_count_of_diffs</t>
+  </si>
+  <si>
+    <t>lse</t>
+  </si>
+  <si>
+    <t>rest_count_of_diffs</t>
+  </si>
+  <si>
+    <t>st_per_growth</t>
+  </si>
+  <si>
     <t>lct</t>
   </si>
   <si>
-    <t>xsga_std</t>
-  </si>
-  <si>
-    <t>xopr</t>
-  </si>
-  <si>
-    <t>xacc_std</t>
-  </si>
-  <si>
-    <t>caps</t>
-  </si>
-  <si>
-    <t>seq</t>
-  </si>
-  <si>
-    <t>ceq</t>
-  </si>
-  <si>
-    <t>sstk_std</t>
-  </si>
-  <si>
-    <t>dp</t>
-  </si>
-  <si>
-    <t>rest_sum_diff</t>
-  </si>
-  <si>
-    <t>sec_trt1m_std</t>
-  </si>
-  <si>
-    <t>sstk</t>
-  </si>
-  <si>
-    <t>wcap</t>
+    <t>gp</t>
+  </si>
+  <si>
+    <t>dilavx_std</t>
+  </si>
+  <si>
+    <t>rect_std</t>
+  </si>
+  <si>
+    <t>dltr_std</t>
   </si>
   <si>
     <t>xopr_std</t>
   </si>
   <si>
-    <t>pi_std</t>
-  </si>
-  <si>
-    <t>rest_count</t>
-  </si>
-  <si>
-    <t>lse</t>
-  </si>
-  <si>
-    <t>fopo_std</t>
-  </si>
-  <si>
-    <t>cogs_std</t>
-  </si>
-  <si>
-    <t>ppegt</t>
-  </si>
-  <si>
-    <t>rest_a_count_of_diffs</t>
-  </si>
-  <si>
-    <t>gp</t>
-  </si>
-  <si>
-    <t>aoloch</t>
-  </si>
-  <si>
-    <t>at_std</t>
-  </si>
-  <si>
-    <t>at</t>
-  </si>
-  <si>
-    <t>icapt</t>
-  </si>
-  <si>
-    <t>teq</t>
-  </si>
-  <si>
-    <t>dlc</t>
-  </si>
-  <si>
-    <t>revt</t>
-  </si>
-  <si>
-    <t>intpn</t>
-  </si>
-  <si>
-    <t>ceq_std</t>
-  </si>
-  <si>
-    <t>rest_count_of_diffs</t>
-  </si>
-  <si>
-    <t>ebit</t>
-  </si>
-  <si>
     <t>xsga</t>
   </si>
   <si>
-    <t>lct_std</t>
-  </si>
-  <si>
-    <t>tstk</t>
-  </si>
-  <si>
-    <t>ceqt</t>
-  </si>
-  <si>
-    <t>pi</t>
-  </si>
-  <si>
-    <t>dilavx_std</t>
-  </si>
-  <si>
-    <t>invt_std</t>
-  </si>
-  <si>
-    <t>seq_std</t>
-  </si>
-  <si>
-    <t>invt</t>
-  </si>
-  <si>
-    <t>teq_std</t>
-  </si>
-  <si>
-    <t>tot_tax_std</t>
-  </si>
-  <si>
-    <t>icapt_std</t>
-  </si>
-  <si>
-    <t>re</t>
+    <t>tstk_std</t>
   </si>
 </sst>
 </file>
@@ -518,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -537,13 +510,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.1311975093389946</v>
+        <v>0.1527071160931781</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -551,27 +524,27 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.08476524991430098</v>
+        <v>0.05270773046560662</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0.05936836012536634</v>
+        <v>0.04971417466192256</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -579,13 +552,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0.04496175166378066</v>
+        <v>0.04836849927228697</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -593,27 +566,27 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0.04448085585593663</v>
+        <v>0.04333180818711402</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0.04330364829327429</v>
+        <v>0.03857920496335165</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -621,13 +594,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0.04155522263896471</v>
+        <v>0.03777455353823508</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -635,41 +608,41 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9">
-        <v>0.03908932476392177</v>
+        <v>0.03648722123215089</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10">
-        <v>0.0379425788551238</v>
+        <v>0.03634344269027862</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11">
-        <v>0.03595357638258925</v>
+        <v>0.03099948577841339</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -677,13 +650,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12">
-        <v>0.0347825283721216</v>
+        <v>0.029939295911582</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -697,7 +670,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>0.03238683576569578</v>
+        <v>0.02940931022326146</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -705,27 +678,27 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14">
-        <v>0.03102307902394075</v>
+        <v>0.02802971129560484</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15">
-        <v>0.03088900684995909</v>
+        <v>0.02608164034783204</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -733,41 +706,41 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16">
-        <v>0.02918156654917575</v>
+        <v>0.02590396875357646</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17">
-        <v>0.02914015275028935</v>
+        <v>0.02185509492567017</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18">
-        <v>0.0253438264160008</v>
+        <v>0.02106721312807415</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -775,41 +748,41 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19">
-        <v>0.02469378760480895</v>
+        <v>0.0206081070694835</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20">
-        <v>0.02454081769444991</v>
+        <v>0.02029893548865565</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21">
-        <v>0.02414491915119098</v>
+        <v>0.01928175878266098</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -817,13 +790,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
       </c>
       <c r="C22">
-        <v>0.02392882786457341</v>
+        <v>0.01925306366437383</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -831,13 +804,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
       <c r="C23">
-        <v>0.0233902266769408</v>
+        <v>0.01893172555107008</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -845,27 +818,27 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>25</v>
       </c>
       <c r="C24">
-        <v>0.02289107638151175</v>
+        <v>0.01853714180679634</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="C25">
-        <v>0.02287440902780302</v>
+        <v>0.01752467437758706</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -873,13 +846,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
       </c>
       <c r="C26">
-        <v>0.02260332633689121</v>
+        <v>0.01702308143061048</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -887,13 +860,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
       </c>
       <c r="C27">
-        <v>0.02203483965053024</v>
+        <v>0.01700241946746915</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -901,27 +874,27 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
       </c>
       <c r="C28">
-        <v>0.02153615811663916</v>
+        <v>0.01635374448785916</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
       <c r="C29">
-        <v>0.0204572682330454</v>
+        <v>0.01623119717182976</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -935,7 +908,7 @@
         <v>31</v>
       </c>
       <c r="C30">
-        <v>0.02034944590047191</v>
+        <v>0.01568318366536436</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -943,13 +916,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
       <c r="C31">
-        <v>0.01813984893286448</v>
+        <v>0.01431435953686472</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -957,55 +930,55 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="C32">
-        <v>0.01738871142771284</v>
+        <v>0.01410872410330963</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33">
-        <v>0.01733681753053857</v>
+        <v>0.012630089981958</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34">
-        <v>0.0166728864170848</v>
+        <v>0.01187474146296748</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
         <v>36</v>
       </c>
       <c r="C35">
-        <v>0.01640542831968089</v>
+        <v>0.01156742718934279</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1013,13 +986,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>37</v>
       </c>
       <c r="C36">
-        <v>0.01513574990217075</v>
+        <v>0.01122832853933041</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -1027,13 +1000,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>38</v>
       </c>
       <c r="C37">
-        <v>0.01512782779687607</v>
+        <v>0.01119838196101883</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1041,141 +1014,15 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
         <v>39</v>
       </c>
       <c r="C38">
-        <v>0.01417570923072858</v>
+        <v>0.01118596017342582</v>
       </c>
       <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1">
-        <v>22</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39">
-        <v>0.01379666222162135</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1">
-        <v>8</v>
-      </c>
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-      <c r="C40">
-        <v>0.01356600908861781</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1">
-        <v>18</v>
-      </c>
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41">
-        <v>0.01342270523402798</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1">
-        <v>33</v>
-      </c>
-      <c r="B42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42">
-        <v>0.0125181251162253</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1">
-        <v>17</v>
-      </c>
-      <c r="B43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43">
-        <v>0.01203810800814309</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1">
-        <v>37</v>
-      </c>
-      <c r="B44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44">
-        <v>0.01171950404716122</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1">
-        <v>38</v>
-      </c>
-      <c r="B45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45">
-        <v>0.01152243565755262</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1">
-        <v>15</v>
-      </c>
-      <c r="B46" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46">
-        <v>0.01112284749121236</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1">
-        <v>25</v>
-      </c>
-      <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47">
-        <v>0.01112245010641218</v>
-      </c>
-      <c r="D47">
         <v>1</v>
       </c>
     </row>

</xml_diff>